<commit_message>
Update excel files and kenote file
</commit_message>
<xml_diff>
--- a/paper/fse21/img/figure9.xlsx
+++ b/paper/fse21/img/figure9.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yundongjun/PLRG/safe/paper/fse21/img/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C68B36-81AB-274B-A2BB-098720434225}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C180964-A098-7848-A051-72E4E4CB61F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="480" windowWidth="35840" windowHeight="20340" activeTab="2" xr2:uid="{816F6371-1B19-2342-BF92-F3A5FD9288FC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="2" xr2:uid="{816F6371-1B19-2342-BF92-F3A5FD9288FC}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="3" r:id="rId1"/>
@@ -2067,7 +2067,7 @@
         <c:axId val="1444397295"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="20"/>
+          <c:max val="16"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -2168,12 +2168,13 @@
         <c:crossAx val="1443977407"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="4"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="1443977407"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="20"/>
+          <c:max val="16"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -2274,6 +2275,7 @@
         <c:crossAx val="1444397295"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="4"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -3975,13 +3977,13 @@
                   <c:v>9999</c:v>
                 </c:pt>
                 <c:pt idx="257">
-                  <c:v>5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="258">
                   <c:v>9999</c:v>
                 </c:pt>
                 <c:pt idx="259">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="260">
                   <c:v>9999</c:v>
@@ -4072,7 +4074,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22.567296678121419</c:v>
+                  <c:v>21.9229667812142</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4136,7 +4138,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>62.5</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4180,7 +4182,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="0"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -4213,7 +4215,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="0"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
@@ -4264,6 +4266,7 @@
         <c:crossAx val="1443977407"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="5"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="1443977407"/>
@@ -5534,15 +5537,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>291327</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>12289</xdr:rowOff>
+      <xdr:colOff>335774</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>221839</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>1644</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>221474</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>226277</xdr:rowOff>
+      <xdr:rowOff>221839</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5554,7 +5557,7 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks noChangeAspect="1"/>
+          <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -5576,12 +5579,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.47627</cdr:x>
-      <cdr:y>0.26167</cdr:y>
+      <cdr:x>0.71855</cdr:x>
+      <cdr:y>0.07639</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.63518</cdr:x>
-      <cdr:y>0.35843</cdr:y>
+      <cdr:x>0.87746</cdr:x>
+      <cdr:y>0.17315</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="'Figure 9 conc'!$K$5">
       <cdr:nvSpPr>
@@ -5595,9 +5598,9 @@
         <cdr:cNvSpPr txBox="1"/>
       </cdr:nvSpPr>
       <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="1681019" y="723070"/>
-          <a:ext cx="560887" cy="267373"/>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="18900000">
+          <a:off x="1971136" y="209552"/>
+          <a:ext cx="435922" cy="265432"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -5651,9 +5654,9 @@
         <cdr:cNvSpPr txBox="1"/>
       </cdr:nvSpPr>
       <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="2564430" y="1928169"/>
-          <a:ext cx="560887" cy="267373"/>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="21360000">
+          <a:off x="1993072" y="1914178"/>
+          <a:ext cx="435922" cy="265432"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -5694,15 +5697,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>86352</xdr:colOff>
+      <xdr:colOff>86350</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>74146</xdr:rowOff>
+      <xdr:rowOff>74145</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>754862</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>899150</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>56382</xdr:rowOff>
+      <xdr:rowOff>74145</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5714,7 +5717,7 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks noChangeAspect="1"/>
+          <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -5736,12 +5739,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.58414</cdr:x>
-      <cdr:y>0.1732</cdr:y>
+      <cdr:x>0.72303</cdr:x>
+      <cdr:y>0.10607</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.74305</cdr:x>
-      <cdr:y>0.26996</cdr:y>
+      <cdr:x>0.88194</cdr:x>
+      <cdr:y>0.20283</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="'Figure 9'!$K$5">
       <cdr:nvSpPr>
@@ -5755,9 +5758,9 @@
         <cdr:cNvSpPr txBox="1"/>
       </cdr:nvSpPr>
       <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="2074838" y="478348"/>
-          <a:ext cx="564443" cy="267238"/>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="18900000">
+          <a:off x="1983413" y="290971"/>
+          <a:ext cx="435922" cy="265432"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -5777,7 +5780,7 @@
               <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
             </a:rPr>
             <a:pPr/>
-            <a:t>y=2.50x</a:t>
+            <a:t>y=1.00x</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="800">
             <a:solidFill>
@@ -5792,12 +5795,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.74166</cdr:x>
-      <cdr:y>0.33825</cdr:y>
+      <cdr:x>0.76944</cdr:x>
+      <cdr:y>0.26649</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.90057</cdr:x>
-      <cdr:y>0.43501</cdr:y>
+      <cdr:x>0.92835</cdr:x>
+      <cdr:y>0.36325</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="'Figure 9'!$K$3">
       <cdr:nvSpPr>
@@ -5811,9 +5814,9 @@
         <cdr:cNvSpPr txBox="1"/>
       </cdr:nvSpPr>
       <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="2634358" y="934194"/>
-          <a:ext cx="564443" cy="267238"/>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="19140000">
+          <a:off x="2110722" y="731038"/>
+          <a:ext cx="435921" cy="265432"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -5833,7 +5836,7 @@
               <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
             </a:rPr>
             <a:pPr/>
-            <a:t>y=0.90x</a:t>
+            <a:t>y=0.88x</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="800">
             <a:solidFill>
@@ -9698,7 +9701,7 @@
             <v>2</v>
           </cell>
           <cell r="X260">
-            <v>5</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="262">
@@ -9709,7 +9712,7 @@
             <v>2</v>
           </cell>
           <cell r="X262">
-            <v>4</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="265">
@@ -10072,8 +10075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC63B65D-BE85-5340-8B51-43D75C4CB2E6}">
   <dimension ref="A1:K272"/>
   <sheetViews>
-    <sheetView topLeftCell="A257" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -21728,7 +21731,7 @@
       </c>
       <c r="I260">
         <f>IF([1]abs!X260="","",[1]abs!X260)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J260" s="7">
         <f t="shared" ref="J260:J271" si="18">IF($G260="","",IF($G260=0,1,($G260-H260)/$G260))</f>
@@ -21736,7 +21739,7 @@
       </c>
       <c r="K260" s="7">
         <f t="shared" ref="K260:K271" si="19">IF($G260="","",IF($G260=0,1,($G260-I260)/$G260))</f>
-        <v>0.16666666666666666</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="261" spans="1:11">
@@ -21818,7 +21821,7 @@
       </c>
       <c r="I262">
         <f>IF([1]abs!X262="","",[1]abs!X262)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J262" s="7">
         <f t="shared" si="18"/>
@@ -21826,7 +21829,7 @@
       </c>
       <c r="K262" s="7">
         <f t="shared" si="19"/>
-        <v>0.33333333333333331</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="263" spans="1:11">
@@ -22253,11 +22256,11 @@
       </c>
       <c r="I272">
         <f>SUM(I3:I271)</f>
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="J272" s="7">
         <f>1-I272/H272</f>
-        <v>0.22653721682847894</v>
+        <v>0.24271844660194175</v>
       </c>
     </row>
   </sheetData>
@@ -22274,15 +22277,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EB64A9D-80DB-D343-9B0B-E4454B8ECBC9}">
   <dimension ref="A1:K272"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView topLeftCell="G10" zoomScale="400" zoomScaleNormal="400" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -28017,6 +28020,10 @@
       </c>
     </row>
     <row r="272" spans="1:5">
+      <c r="B272" s="9">
+        <f>COUNTIFS(B3:B271,"&gt;0",B3:B271,"&lt;9999")</f>
+        <v>26</v>
+      </c>
       <c r="D272" s="5"/>
     </row>
   </sheetData>
@@ -28033,8 +28040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{098AB617-AF3F-554F-94B6-FBBFE57413D7}">
   <dimension ref="A1:K272"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="159" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="F10" zoomScale="400" zoomScaleNormal="400" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -28105,18 +28112,18 @@
       </c>
       <c r="F3" s="3">
         <f>AVERAGEIF(D3:D271, "&lt;&gt;*")</f>
-        <v>0.90269186712485672</v>
+        <v>0.87691867124856804</v>
       </c>
       <c r="H3" s="3">
         <v>25</v>
       </c>
       <c r="I3" s="3">
         <f>H3*F3</f>
-        <v>22.567296678121419</v>
+        <v>21.9229667812142</v>
       </c>
       <c r="K3" t="str">
         <f>"y="&amp;TEXT(F3,"0.00")&amp;"x"</f>
-        <v>y=0.90x</v>
+        <v>y=0.88x</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -28171,18 +28178,18 @@
       </c>
       <c r="F5" s="3">
         <f>MAX(D3:D271)</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="H5" s="3">
         <v>25</v>
       </c>
       <c r="I5" s="3">
         <f>H5*F5</f>
-        <v>62.5</v>
+        <v>25</v>
       </c>
       <c r="K5" t="str">
         <f>"y="&amp;TEXT(F5,"0.00")&amp;"x"</f>
-        <v>y=2.50x</v>
+        <v>y=1.00x</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -28231,7 +28238,7 @@
       </c>
       <c r="F7" s="5">
         <f>AVERAGE(E3:E271)</f>
-        <v>0.44871794871794873</v>
+        <v>0.48076923076923078</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -33536,15 +33543,15 @@
       </c>
       <c r="C260" s="9">
         <f>IF(data!I260="",9999,data!I260)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D260" s="5">
         <f t="shared" ref="D260:D271" si="8">IF(OR(B260=9999,C260=9999),"",IFERROR(C260/B260,""))</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="E260">
         <f t="shared" ref="E260:E271" si="9">IF(AND(B260&lt;&gt;9999,C260&lt;&gt;9999),B260-C260,"")</f>
-        <v>-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="261" spans="1:5">
@@ -33578,15 +33585,15 @@
       </c>
       <c r="C262" s="9">
         <f>IF(data!I262="",9999,data!I262)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D262" s="5">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E262">
         <f t="shared" si="9"/>
-        <v>-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="263" spans="1:5">

</xml_diff>